<commit_message>
refactor excel reading code
</commit_message>
<xml_diff>
--- a/src/main/resources/testFiles/credentials.xlsx
+++ b/src/main/resources/testFiles/credentials.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20398"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F23E18C-EC64-4D0A-9E75-793CC6CC5217}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65CAF03B-2860-4B68-928B-727BA26E1DAA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,17 +21,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>keqnlsk</t>
   </si>
   <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
     <t>Rahul</t>
   </si>
   <si>
@@ -44,16 +38,10 @@
     <t>Pooja</t>
   </si>
   <si>
-    <t>Rahul123</t>
-  </si>
-  <si>
-    <t>Laxman222</t>
-  </si>
-  <si>
-    <t>Pooja444</t>
-  </si>
-  <si>
-    <t>Anjuli333</t>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Age</t>
   </si>
 </sst>
 </file>
@@ -77,7 +65,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -85,12 +73,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -374,53 +381,54 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="40.85546875" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="2">
+        <v>29.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B3" s="2">
+        <v>30.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B4" s="2">
+        <v>31.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
+      <c r="B5" s="2">
+        <v>32.299999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>